<commit_message>
Improvements on importing non-PeMS databases
</commit_message>
<xml_diff>
--- a/inputs/ids_per_segtype/Weaving.xlsx
+++ b/inputs/ids_per_segtype/Weaving.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lstaichakcarvalh\Documents\Python_files\PeMS_DataExtractor\inputs\ids_per_segtype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lstaichakcarvalh\Documents\Python_files\PeMSDataExtractor\inputs\ids_per_segtype\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -371,7 +371,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +400,9 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>101</v>
+      </c>
       <c r="C2" s="3">
         <v>95</v>
       </c>
@@ -417,7 +419,9 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>103</v>
+      </c>
       <c r="C3" s="3">
         <v>97</v>
       </c>
@@ -434,7 +438,9 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>104</v>
+      </c>
       <c r="C4" s="1">
         <v>98</v>
       </c>
@@ -448,8 +454,12 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>105</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
@@ -458,7 +468,12 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>106</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>

</xml_diff>